<commit_message>
Updated readme installation instructions
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtc0030/Documents/Projects/HAB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtc0030/Documents/Projects/HAB/ros-hab-dcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B376B1B6-18B6-D341-8865-CAFF0CFDD883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA470B1-05F0-0C4A-8DAA-34A038C47F34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{9E5CD0A4-BAAD-3342-BAB6-1E57A22FEC73}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="157">
   <si>
     <t>Component</t>
   </si>
@@ -482,9 +482,6 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/4298</t>
-  </si>
-  <si>
-    <t>Shipping</t>
   </si>
   <si>
     <t>Amazon (Tape and GPS)</t>
@@ -674,67 +671,7 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1078,7 +1015,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1368,7 +1305,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>21</v>
@@ -1400,7 +1337,7 @@
         <v>7.95</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>25</v>
@@ -2073,7 +2010,7 @@
         <v>3.77</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>21</v>
@@ -2105,7 +2042,7 @@
         <v>1.29</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>21</v>
@@ -2263,13 +2200,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G34">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="On Hand">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="On Hand">
       <formula>NOT(ISERROR(SEARCH("On Hand",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Shipping">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Shipping">
       <formula>NOT(ISERROR(SEARCH("Shipping",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Hold">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Hold">
       <formula>NOT(ISERROR(SEARCH("Hold",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2290,7 +2227,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2442,7 +2379,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="7">
         <v>44145</v>
@@ -2462,7 +2399,7 @@
         <v>118</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="7">
         <v>44145</v>
@@ -2470,16 +2407,19 @@
       <c r="E9" s="7">
         <v>44151</v>
       </c>
+      <c r="F9" s="7">
+        <v>44152</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="7">
         <v>44145</v>
@@ -2487,13 +2427,16 @@
       <c r="E10" s="7">
         <v>44151</v>
       </c>
+      <c r="F10" s="7">
+        <v>44152</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" s="7">
         <v>44145</v>

</xml_diff>